<commit_message>
~ Pasta de trabalho actualizada.
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -148,9 +148,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -159,6 +156,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -457,8 +457,8 @@
   <dimension ref="A1:Q245"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
+      <pane ySplit="1" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M159" sqref="M159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -497,22 +497,22 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -10823,10 +10823,10 @@
       </c>
     </row>
     <row r="243" spans="1:17">
-      <c r="B243" s="8" t="s">
+      <c r="B243" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C243" s="9" t="s">
+      <c r="C243" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D243" s="3"/>
@@ -10864,16 +10864,16 @@
       </c>
     </row>
     <row r="244" spans="1:17">
-      <c r="C244" s="7" t="s">
+      <c r="C244" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D244" s="7"/>
-      <c r="E244" s="7"/>
-      <c r="F244" s="7"/>
-      <c r="G244" s="7"/>
-      <c r="H244" s="7"/>
-      <c r="I244" s="7"/>
-      <c r="J244" s="7"/>
+      <c r="D244" s="10"/>
+      <c r="E244" s="10"/>
+      <c r="F244" s="10"/>
+      <c r="G244" s="10"/>
+      <c r="H244" s="10"/>
+      <c r="I244" s="10"/>
+      <c r="J244" s="10"/>
       <c r="K244" t="s">
         <v>6</v>
       </c>
@@ -10906,27 +10906,27 @@
         <v>8</v>
       </c>
       <c r="L245">
-        <f>(L243/L242)*100</f>
+        <f t="shared" ref="L245:Q245" si="24">(L243/L242)*100</f>
         <v>45</v>
       </c>
       <c r="M245">
-        <f>(M243/M242)*100</f>
+        <f t="shared" si="24"/>
         <v>65.476190476190482</v>
       </c>
       <c r="N245">
-        <f>(N243/N242)*100</f>
+        <f t="shared" si="24"/>
         <v>61.904761904761905</v>
       </c>
       <c r="O245">
-        <f>(O243/O242)*100</f>
+        <f t="shared" si="24"/>
         <v>64.285714285714292</v>
       </c>
       <c r="P245" s="4">
-        <f>(P243/P242)*100</f>
+        <f t="shared" si="24"/>
         <v>73.80952380952381</v>
       </c>
       <c r="Q245">
-        <f>(Q243/Q242)*100</f>
+        <f t="shared" si="24"/>
         <v>60.714285714285708</v>
       </c>
     </row>

</xml_diff>